<commit_message>
Using Custom-sort to Sort Multiple Columns Within a Table
</commit_message>
<xml_diff>
--- a/Section 4/34. Custom Number Formatting/31.+Assigning+Custom+Formats+-+Exercise+-+Unsolved.xlsx
+++ b/Section 4/34. Custom Number Formatting/31.+Assigning+Custom+Formats+-+Exercise+-+Unsolved.xlsx
@@ -1,19 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17030"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2DBA29F-01A2-4715-964D-DB2C1D4A9974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795"/>
+    <workbookView xWindow="28680" yWindow="270" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exercise" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -37,10 +49,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General\ \+"/>
     <numFmt numFmtId="165" formatCode="General\ \x"/>
+    <numFmt numFmtId="166" formatCode="0\ \д\н\і\в;"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -146,10 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -157,14 +167,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -175,24 +192,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,11 +517,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:H11"/>
+      <selection activeCell="I19" sqref="H19:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,152 +535,125 @@
     <col min="8" max="8" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="J2" s="19" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="J2" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="J3" s="20"/>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="13">
+    <row r="3" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="J3" s="10"/>
+    </row>
+    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="11">
         <v>1</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="21" t="s">
+      <c r="C5" s="13"/>
+      <c r="D5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="13">
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+    </row>
+    <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+    </row>
+    <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="2:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="11">
         <v>2</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16" t="s">
+      <c r="C9" s="13"/>
+      <c r="D9" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H18" s="11"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+    </row>
+    <row r="10" spans="2:10" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+    </row>
+    <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -698,8 +677,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B3:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -712,56 +691,36 @@
     <col min="3" max="3" width="5" customWidth="1"/>
     <col min="4" max="4" width="7.140625" customWidth="1"/>
     <col min="5" max="5" width="7.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="6.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="6"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="7"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="7"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="10"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D7" s="10"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="10"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D8" s="10"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="10"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="10"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="10"/>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="3"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="3"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>